<commit_message>
added phrase frequency vals to URL spreadsheet
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/AllUniqueTranscriptionURL.xlsx
+++ b/MechanicalTurkStuff/AllUniqueTranscriptionURL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="13200" yWindow="2860" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve"> Input.audioURL</t>
   </si>
@@ -77,6 +77,60 @@
   </si>
   <si>
     <t xml:space="preserve"> http://ani.pe/jenee/A.17.135.wav</t>
+  </si>
+  <si>
+    <t>eh nice cole dower</t>
+  </si>
+  <si>
+    <t>a nice coal dower</t>
+  </si>
+  <si>
+    <t>on ice coal dower</t>
+  </si>
+  <si>
+    <t>an ice kohl dower</t>
+  </si>
+  <si>
+    <t>an ice cole dower</t>
+  </si>
+  <si>
+    <t>an ice coal dower</t>
+  </si>
+  <si>
+    <t>an aye scold hour</t>
+  </si>
+  <si>
+    <t>a nye scold hour</t>
+  </si>
+  <si>
+    <t>a nigh scold our</t>
+  </si>
+  <si>
+    <t>on ice cold hour</t>
+  </si>
+  <si>
+    <t>an ice-cold hour</t>
+  </si>
+  <si>
+    <t>an eye scold our</t>
+  </si>
+  <si>
+    <t>a nye scold our</t>
+  </si>
+  <si>
+    <t>a nice cold our</t>
+  </si>
+  <si>
+    <t>an ice-cold our</t>
+  </si>
+  <si>
+    <t>an ice cold our</t>
+  </si>
+  <si>
+    <t>calculated_Freq</t>
+  </si>
+  <si>
+    <t>recording script</t>
   </si>
 </sst>
 </file>
@@ -469,110 +523,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>259836</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>7747545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>2806985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>807375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>808536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>826911</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>996702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>7608364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>8011331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>2911102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>866031</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>866031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>1294559</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>8009974</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>8253272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>1267641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>1332638</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>